<commit_message>
alle orte in einem
</commit_message>
<xml_diff>
--- a/Data/Samstag/joined_Samstag_coord_nn.xlsx
+++ b/Data/Samstag/joined_Samstag_coord_nn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Desktop\git_folder\DataScienceProject\Data\Samstag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC13FC78-AAD1-4E65-86AC-2837D92AD191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40AE5D2-BD74-4B27-8BBF-0DCE9622CA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>ADRESSE</t>
   </si>
   <si>
-    <t>Longitude_x</t>
-  </si>
-  <si>
-    <t>Latitude_x</t>
-  </si>
-  <si>
     <t>Kärnthnerthor</t>
   </si>
   <si>
@@ -52,30 +46,6 @@
     <t>Laxenburger Allee</t>
   </si>
   <si>
-    <t>04., Argentinierstraße 39</t>
-  </si>
-  <si>
-    <t>10., Laxenburger Straße 219</t>
-  </si>
-  <si>
-    <t>16.28518125227009</t>
-  </si>
-  <si>
-    <t>16.374740257710602</t>
-  </si>
-  <si>
-    <t>16.36272365048848</t>
-  </si>
-  <si>
-    <t>48.16392472344249</t>
-  </si>
-  <si>
-    <t>48.19188809841415</t>
-  </si>
-  <si>
-    <t>48.15097732579337</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -109,12 +79,6 @@
     <t>https://geohack.toolforge.org/geohack.php?pagename=K.k._Polytechnisches_Institut&amp;language=de&amp;params=48.198888_N_16.369912_E_region:AT-9_type:landmark</t>
   </si>
   <si>
-    <t>schen Jnstituts 1. Hof, Direk=</t>
-  </si>
-  <si>
-    <t>tionstiege, 1. Stock=</t>
-  </si>
-  <si>
     <t>Jn Gebäude des voltechi=schen Jnstituts 1. Hof, Direk=tionstiege, 1. Stock=</t>
   </si>
   <si>
@@ -124,14 +88,38 @@
     <t>NEUE_NAMEN</t>
   </si>
   <si>
-    <t>KulturwikiOGD</t>
+    <t>04., Taubstummengasse 13-17</t>
+  </si>
+  <si>
+    <t>04., Favoritenstraße 15</t>
+  </si>
+  <si>
+    <t>04., Favoritenstraße 16</t>
+  </si>
+  <si>
+    <t>https://www.geschichtewiki.wien.gv.at/Theresianische_Akademie_(Geb%C3%A4ude)</t>
+  </si>
+  <si>
+    <t>https://www.geschichtewiki.wien.gv.at/Taubstummeninstitut</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>QGIS - Estimation</t>
+  </si>
+  <si>
+    <t>mittel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +131,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -191,40 +185,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -260,6 +226,35 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -274,15 +269,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E7F177A-FAD6-4711-916D-917DCE8EAB7B}" name="Table1" displayName="Table1" ref="A1:H9" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E7F177A-FAD6-4711-916D-917DCE8EAB7B}" name="Table1" displayName="Table1" ref="A1:H9" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:H9" xr:uid="{1E7F177A-FAD6-4711-916D-917DCE8EAB7B}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{99B5889C-43EB-44E4-8EC4-039802BDB39F}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{99B5889C-43EB-44E4-8EC4-039802BDB39F}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{1F072E69-C905-4F28-99E0-DB4C12E692C7}" name="NEUE_NAMEN"/>
     <tableColumn id="3" xr3:uid="{E683E16D-055D-4C14-87B5-66AB0F41405D}" name="ADRESSE"/>
     <tableColumn id="8" xr3:uid="{00F977C2-4F98-41D4-94DC-B5303AA70EDE}" name="Sicherheit"/>
-    <tableColumn id="4" xr3:uid="{ECB13CEC-F1F4-4A0F-AD2E-B4B0AEFD4A0A}" name="Longitude_x"/>
-    <tableColumn id="5" xr3:uid="{A6C9F7B1-99B0-43D6-ABB2-5D27D1BC668E}" name="Latitude_x"/>
+    <tableColumn id="4" xr3:uid="{ECB13CEC-F1F4-4A0F-AD2E-B4B0AEFD4A0A}" name="Longitude"/>
+    <tableColumn id="5" xr3:uid="{A6C9F7B1-99B0-43D6-ABB2-5D27D1BC668E}" name="Latitude"/>
     <tableColumn id="6" xr3:uid="{169C76B8-0C93-43B6-A9D0-9E92BD41885E}" name="Quelle"/>
     <tableColumn id="7" xr3:uid="{2F70EED4-F870-42DA-AC64-8ECBD2AB4F23}" name="URL"/>
   </tableColumns>
@@ -577,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,28 +591,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -625,13 +620,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>16.370534457671599</v>
@@ -640,10 +635,10 @@
         <v>48.203303433951199</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -651,13 +646,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
         <v>16.369911999999999</v>
@@ -666,10 +661,10 @@
         <v>48.198887999999997</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -677,10 +672,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>16.369911999999999</v>
+      </c>
+      <c r="F4">
+        <v>48.198887999999997</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -688,19 +698,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>16.3709411171927</v>
+      </c>
+      <c r="F5">
+        <v>48.195140442994003</v>
+      </c>
+      <c r="G5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
+      <c r="H5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -708,19 +724,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
+      <c r="E6">
+        <v>16.3714736393609</v>
+      </c>
+      <c r="F6">
+        <v>48.193537549633099</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -728,19 +750,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>16.3714736393609</v>
+      </c>
+      <c r="F7">
+        <v>48.193537549633099</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -748,10 +776,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>16.379925897949999</v>
+      </c>
+      <c r="F8">
+        <v>48.185791939397014</v>
+      </c>
+      <c r="G8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -759,22 +799,26 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
+      <c r="E9">
+        <v>16.374092267197891</v>
+      </c>
+      <c r="F9">
+        <v>48.182660301764052</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F14" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>